<commit_message>
upload and fix files
</commit_message>
<xml_diff>
--- a/python-excel-how-objects-work-solutions.xlsx
+++ b/python-excel-how-objects-work-solutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Documents\GitHub\blog-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32213310-EE47-44F3-8C58-81B831E8699B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712AE0E4-9370-4177-8621-0D25951AD8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="18915" windowHeight="12676" activeTab="1" xr2:uid="{5126D4A5-837A-4E20-A2E6-9D659AA5F7AC}"/>
   </bookViews>
@@ -38,9 +38,8 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="2">
+  <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -51,35 +50,11 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="2">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="2"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="4"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="2">
-    <bk>
-      <rc t="2" v="0"/>
-    </bk>
-    <bk>
-      <rc t="2" v="1"/>
-    </bk>
-  </valueMetadata>
 </metadata>
 </file>
 
@@ -96,22 +71,13 @@
 points.columns</code>
   </pythonScript>
   <pythonScript>
-    <code>points_dict = points.to_dict()</code>
-  </pythonScript>
-  <pythonScript>
-    <code># Update Lebron's score
-points_dict['LeBron'] = 38927
-# Add Dirk to dict
-points_dict['Dirk'] = 31560</code>
-  </pythonScript>
-  <pythonScript>
-    <code>points = pd.DataFrame(points_dict)</code>
+    <code>points_array = points['points'].to_numpy()</code>
   </pythonScript>
 </pythonScripts>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>player</t>
   </si>
@@ -186,19 +152,28 @@
   </si>
   <si>
     <t>birth_state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="26"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,8 +196,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -238,186 +216,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
-  <rv s="0">
-    <v>1</v>
-    <v>Entity</v>
-    <v>LeBron</v>
-    <v>Kareem</v>
-    <v>Karl</v>
-    <v>Kobe</v>
-    <v>Michael</v>
-  </rv>
-  <rv s="1">
-    <v>1</v>
-    <v>Entity</v>
-    <v>38923</v>
-    <v>38387</v>
-    <v>36928</v>
-    <v>33643</v>
-    <v>32292</v>
-  </rv>
-  <rv s="2">
-    <v>0</v>
-    <v>Entity</v>
-    <v>0</v>
-    <v>1</v>
-  </rv>
-  <rv s="3">
-    <fb>0</fb>
-    <v>2</v>
-  </rv>
-  <rv s="4">
-    <fb>0</fb>
-    <v>&lt;class 'NoneType'&gt;</v>
-    <v>NoneType</v>
-    <v>None</v>
-    <v>3</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
-  <s t="_entity">
-    <k n="_Display" t="spb"/>
-    <k n="_DisplayString" t="s"/>
-    <k n="0" t="s"/>
-    <k n="1" t="s"/>
-    <k n="2" t="s"/>
-    <k n="3" t="s"/>
-    <k n="4" t="s"/>
-  </s>
-  <s t="_entity">
-    <k n="_Display" t="spb"/>
-    <k n="_DisplayString" t="s"/>
-    <k n="0" t="i"/>
-    <k n="1" t="i"/>
-    <k n="2" t="i"/>
-    <k n="3" t="i"/>
-    <k n="4" t="i"/>
-  </s>
-  <s t="_entity">
-    <k n="_Display" t="spb"/>
-    <k n="_DisplayString" t="s"/>
-    <k n="first_name" t="r"/>
-    <k n="points" t="r"/>
-  </s>
-  <s t="_formattednumber">
-    <k n="_Format" t="spb"/>
-  </s>
-  <s t="_python">
-    <k n="Python_type" t="s"/>
-    <k n="Python_typeName" t="s"/>
-    <k n="Python_str" t="s"/>
-    <k n="preview" t="r"/>
-  </s>
-</rvStructures>
-</file>
-
-<file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
-<supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
-  <spbArrays count="2">
-    <a count="4">
-      <v t="s">first_name</v>
-      <v t="s">points</v>
-      <v t="s">_DisplayString</v>
-      <v t="s">_Display</v>
-    </a>
-    <a count="7">
-      <v t="s">0</v>
-      <v t="s">1</v>
-      <v t="s">2</v>
-      <v t="s">3</v>
-      <v t="s">4</v>
-      <v t="s">_DisplayString</v>
-      <v t="s">_Display</v>
-    </a>
-  </spbArrays>
-  <spbData count="3">
-    <spb s="0">
-      <v>0</v>
-    </spb>
-    <spb s="0">
-      <v>1</v>
-    </spb>
-    <spb s="1">
-      <v>1</v>
-    </spb>
-  </spbData>
-</supportingPropertyBags>
-</file>
-
-<file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="2">
-  <s>
-    <k n="^Order" t="spba"/>
-  </s>
-  <s>
-    <k n="_Self" t="i"/>
-  </s>
-</spbStructures>
-</file>
-
-<file path=xl/richData/richStyles.xml><?xml version="1.0" encoding="utf-8"?>
-<richStyleSheet xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <dxfs count="1">
-    <x:dxf>
-      <x:numFmt numFmtId="0" formatCode="General"/>
-    </x:dxf>
-  </dxfs>
-  <richProperties>
-    <rPr n="NumberFormat" t="s"/>
-  </richProperties>
-  <richStyles>
-    <rSty dxfid="0">
-      <rpv i="0">0;-0;* "None"</rpv>
-    </rSty>
-  </richStyles>
-</richStyleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -989,10 +787,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A70547-EFC7-42EC-9C11-814561E2AD5C}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="34.15" x14ac:dyDescent="1.05"/>
@@ -1040,9 +838,9 @@
       <c r="B4">
         <v>36928</v>
       </c>
-      <c r="D4" t="e" cm="1" vm="1">
-        <f t="array" ref="D4">_xlfn._xlws.PY(3,0)</f>
-        <v>#VALUE!</v>
+      <c r="D4" cm="1">
+        <f t="array" ref="D4:D8">_xlfn._xlws.PY(3,0)</f>
+        <v>38923</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="1.05">
@@ -1052,6 +850,9 @@
       <c r="B5">
         <v>33643</v>
       </c>
+      <c r="D5">
+        <v>38387</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="1.05">
       <c r="A6" t="s">
@@ -1060,94 +861,23 @@
       <c r="B6">
         <v>32292</v>
       </c>
-      <c r="D6" cm="1" vm="2">
-        <f t="array" ref="D6">_xlfn._xlws.PY(4,1)</f>
-        <v>0</v>
+      <c r="D6">
+        <v>36928</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="1.05">
+      <c r="D7">
+        <v>33643</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="1.05">
-      <c r="A8" t="str" cm="1">
-        <f t="array" ref="A8:D13">_xlfn._xlws.PY(5,0)</f>
-        <v>first_name</v>
-      </c>
-      <c r="B8" t="str">
-        <v>points</v>
-      </c>
-      <c r="C8" t="str">
-        <v>LeBron</v>
-      </c>
-      <c r="D8" t="str">
-        <v>Dirk</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="1.05">
-      <c r="A9" t="str">
-        <v>LeBron</v>
-      </c>
-      <c r="B9">
-        <v>38923</v>
-      </c>
-      <c r="C9">
-        <v>38927</v>
-      </c>
-      <c r="D9">
-        <v>31560</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="1.05">
-      <c r="A10" t="str">
-        <v>Kareem</v>
-      </c>
-      <c r="B10">
-        <v>38387</v>
-      </c>
-      <c r="C10">
-        <v>38927</v>
-      </c>
-      <c r="D10">
-        <v>31560</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="1.05">
-      <c r="A11" t="str">
-        <v>Karl</v>
-      </c>
-      <c r="B11">
-        <v>36928</v>
-      </c>
-      <c r="C11">
-        <v>38927</v>
-      </c>
-      <c r="D11">
-        <v>31560</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="1.05">
-      <c r="A12" t="str">
-        <v>Kobe</v>
-      </c>
-      <c r="B12">
-        <v>33643</v>
-      </c>
-      <c r="C12">
-        <v>38927</v>
-      </c>
-      <c r="D12">
-        <v>31560</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="1.05">
-      <c r="A13" t="str">
-        <v>Michael</v>
-      </c>
-      <c r="B13">
+      <c r="D8">
         <v>32292</v>
       </c>
-      <c r="C13">
-        <v>38927</v>
-      </c>
-      <c r="D13">
-        <v>31560</v>
+    </row>
+    <row r="11" spans="1:4" ht="66.400000000000006" x14ac:dyDescent="1.05">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>